<commit_message>
Adding a 'pillar' column to indicator_order/indicator_df to identify calculations groups in HEP and UHC
</commit_message>
<xml_diff>
--- a/data-raw/indicator_order.xlsx
+++ b/data-raw/indicator_order.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\documents\WHO\billionaiRe\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7171C9D3-0723-43FF-B7A9-804A0C2607C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC8516A-B13F-4C32-BD75-AAC6E74EE044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{BB7C0A8F-3E4B-42D2-A48C-0464F3997827}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="278">
   <si>
     <t>SDG 2.2.1</t>
   </si>
@@ -934,6 +934,36 @@
   </si>
   <si>
     <t>unit_transformed</t>
+  </si>
+  <si>
+    <t>pillar</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>RMNCH</t>
+  </si>
+  <si>
+    <t>infec_diseases</t>
+  </si>
+  <si>
+    <t>ncd</t>
+  </si>
+  <si>
+    <t>service_cap_access</t>
+  </si>
+  <si>
+    <t>fin_hardship</t>
+  </si>
+  <si>
+    <t>prepare</t>
+  </si>
+  <si>
+    <t>prevent</t>
+  </si>
+  <si>
+    <t>detect_response</t>
   </si>
 </sst>
 </file>
@@ -1464,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497A527C-AEDB-4138-8664-DD03992C96A6}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1481,7 +1511,7 @@
     <col min="8" max="8" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="9" t="s">
         <v>86</v>
       </c>
@@ -1506,8 +1536,11 @@
       <c r="H1" s="12" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1">
+      <c r="I1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1532,8 +1565,11 @@
       <c r="H2" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1558,8 +1594,11 @@
       <c r="H3" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1584,8 +1623,11 @@
       <c r="H4" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1610,8 +1652,11 @@
       <c r="H5" s="11">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1636,8 +1681,11 @@
       <c r="H6" s="11">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1662,8 +1710,11 @@
       <c r="H7" s="11">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -1688,8 +1739,11 @@
       <c r="H8" s="11">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -1714,8 +1768,11 @@
       <c r="H9" s="11">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -1740,8 +1797,11 @@
       <c r="H10" s="11">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1766,8 +1826,11 @@
       <c r="H11" s="11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -1792,8 +1855,11 @@
       <c r="H12" s="11">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
@@ -1818,8 +1884,11 @@
       <c r="H13" s="11">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -1844,8 +1913,11 @@
       <c r="H14" s="11">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
@@ -1870,8 +1942,11 @@
       <c r="H15" s="11">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -1896,8 +1971,11 @@
       <c r="H16" s="11">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
@@ -1922,8 +2000,11 @@
       <c r="H17" s="11">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
@@ -1948,8 +2029,11 @@
       <c r="H18" s="11">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
         <v>52</v>
       </c>
@@ -1974,8 +2058,11 @@
       <c r="H19" s="11">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
         <v>56</v>
       </c>
@@ -2000,8 +2087,11 @@
       <c r="H20" s="11">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
@@ -2026,8 +2116,11 @@
       <c r="H21" s="11">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="6" t="s">
         <v>16</v>
       </c>
@@ -2052,8 +2145,11 @@
       <c r="H22" s="11">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="7" t="s">
         <v>113</v>
       </c>
@@ -2078,8 +2174,11 @@
       <c r="H23" s="11">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="7" t="s">
         <v>114</v>
       </c>
@@ -2104,8 +2203,11 @@
       <c r="H24" s="11">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="7" t="s">
         <v>115</v>
       </c>
@@ -2130,8 +2232,11 @@
       <c r="H25" s="11">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="7" t="s">
         <v>116</v>
       </c>
@@ -2156,8 +2261,11 @@
       <c r="H26" s="11">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="7" t="s">
         <v>117</v>
       </c>
@@ -2182,8 +2290,11 @@
       <c r="H27" s="11">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="7" t="s">
         <v>140</v>
       </c>
@@ -2208,8 +2319,11 @@
       <c r="H28" s="11">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="7" t="s">
         <v>141</v>
       </c>
@@ -2234,8 +2348,11 @@
       <c r="H29" s="11">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="7" t="s">
         <v>142</v>
       </c>
@@ -2260,8 +2377,11 @@
       <c r="H30" s="11">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="7" t="s">
         <v>143</v>
       </c>
@@ -2286,8 +2406,11 @@
       <c r="H31" s="11">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="7" t="s">
         <v>144</v>
       </c>
@@ -2312,8 +2435,11 @@
       <c r="H32" s="11">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="7" t="s">
         <v>145</v>
       </c>
@@ -2338,8 +2464,11 @@
       <c r="H33" s="11">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="7" t="s">
         <v>146</v>
       </c>
@@ -2364,8 +2493,11 @@
       <c r="H34" s="11">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="7" t="s">
         <v>147</v>
       </c>
@@ -2390,8 +2522,11 @@
       <c r="H35" s="11">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="7" t="s">
         <v>148</v>
       </c>
@@ -2416,8 +2551,11 @@
       <c r="H36" s="11">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="22.5">
+      <c r="I36" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="22.5">
       <c r="A37" s="7" t="s">
         <v>149</v>
       </c>
@@ -2442,8 +2580,11 @@
       <c r="H37" s="11">
         <v>32</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="7" t="s">
         <v>150</v>
       </c>
@@ -2468,8 +2609,11 @@
       <c r="H38" s="11">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="22.5">
+      <c r="I38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="22.5">
       <c r="A39" s="19" t="s">
         <v>155</v>
       </c>
@@ -2494,8 +2638,11 @@
       <c r="H39" s="11">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="19" t="s">
         <v>208</v>
       </c>
@@ -2520,8 +2667,11 @@
       <c r="H40" s="11">
         <v>35</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="19" t="s">
         <v>209</v>
       </c>
@@ -2546,8 +2696,11 @@
       <c r="H41" s="11">
         <v>36</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="19" t="s">
         <v>210</v>
       </c>
@@ -2572,8 +2725,11 @@
       <c r="H42" s="11">
         <v>37</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="19" t="s">
         <v>211</v>
       </c>
@@ -2598,8 +2754,11 @@
       <c r="H43" s="11">
         <v>38</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="19" t="s">
         <v>212</v>
       </c>
@@ -2624,8 +2783,11 @@
       <c r="H44" s="11">
         <v>39</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="19" t="s">
         <v>213</v>
       </c>
@@ -2650,8 +2812,11 @@
       <c r="H45" s="11">
         <v>40</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="19" t="s">
         <v>214</v>
       </c>
@@ -2676,8 +2841,11 @@
       <c r="H46" s="11">
         <v>41</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="19" t="s">
         <v>215</v>
       </c>
@@ -2702,8 +2870,11 @@
       <c r="H47" s="11">
         <v>42</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="19" t="s">
         <v>216</v>
       </c>
@@ -2728,8 +2899,11 @@
       <c r="H48" s="11">
         <v>43</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="19" t="s">
         <v>217</v>
       </c>
@@ -2754,8 +2928,11 @@
       <c r="H49" s="11">
         <v>44</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="19" t="s">
         <v>218</v>
       </c>
@@ -2780,8 +2957,11 @@
       <c r="H50" s="11">
         <v>45</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="19" t="s">
         <v>219</v>
       </c>
@@ -2806,8 +2986,11 @@
       <c r="H51" s="11">
         <v>46</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="I51" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="19" t="s">
         <v>220</v>
       </c>
@@ -2832,8 +3015,11 @@
       <c r="H52" s="11">
         <v>47</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="I52" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="19" t="s">
         <v>221</v>
       </c>
@@ -2858,8 +3044,11 @@
       <c r="H53" s="11">
         <v>48</v>
       </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="I53" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="19" t="s">
         <v>222</v>
       </c>
@@ -2884,8 +3073,11 @@
       <c r="H54" s="11">
         <v>49</v>
       </c>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="I54" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" s="19" t="s">
         <v>223</v>
       </c>
@@ -2910,8 +3102,11 @@
       <c r="H55" s="11">
         <v>50</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="I55" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="19" t="s">
         <v>224</v>
       </c>
@@ -2936,8 +3131,11 @@
       <c r="H56" s="11">
         <v>51</v>
       </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="I56" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="19" t="s">
         <v>225</v>
       </c>
@@ -2962,8 +3160,11 @@
       <c r="H57" s="11">
         <v>52</v>
       </c>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="I57" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="19" t="s">
         <v>226</v>
       </c>
@@ -2988,8 +3189,11 @@
       <c r="H58" s="11">
         <v>53</v>
       </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="I58" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" s="19" t="s">
         <v>227</v>
       </c>
@@ -3014,8 +3218,11 @@
       <c r="H59" s="11">
         <v>54</v>
       </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="I59" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" s="19" t="s">
         <v>228</v>
       </c>
@@ -3040,8 +3247,11 @@
       <c r="H60" s="11">
         <v>55</v>
       </c>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="I60" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="19" t="s">
         <v>229</v>
       </c>
@@ -3066,8 +3276,11 @@
       <c r="H61" s="11">
         <v>56</v>
       </c>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="I61" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="19" t="s">
         <v>230</v>
       </c>
@@ -3091,6 +3304,9 @@
       </c>
       <c r="H62" s="11">
         <v>57</v>
+      </c>
+      <c r="I62" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -3110,12 +3326,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -3332,6 +3542,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4F5669-9080-4211-AAB2-07BF8DFB6BC3}">
   <ds:schemaRefs>
@@ -3341,22 +3557,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2A8D83-3442-4B82-A652-52EBAFE721A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cee211f1-5bf1-4f4b-adf1-18b7c5b9a3a6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C331FB4-7C5E-4701-8F41-17478B6D46F4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3373,4 +3573,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2A8D83-3442-4B82-A652-52EBAFE721A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cee211f1-5bf1-4f4b-adf1-18b7c5b9a3a6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modify indicator_order to add pillar column
</commit_message>
<xml_diff>
--- a/data-raw/indicator_order.xlsx
+++ b/data-raw/indicator_order.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC8516A-B13F-4C32-BD75-AAC6E74EE044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8FD295-B5E5-428A-8395-D5CA4962607E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{BB7C0A8F-3E4B-42D2-A48C-0464F3997827}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{BB7C0A8F-3E4B-42D2-A48C-0464F3997827}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="279">
   <si>
     <t>SDG 2.2.1</t>
   </si>
@@ -965,12 +965,15 @@
   <si>
     <t>detect_response</t>
   </si>
+  <si>
+    <t>comment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1494,24 +1497,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497A527C-AEDB-4138-8664-DD03992C96A6}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="28.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="86.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="11"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="28.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="86.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7265625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="33.81640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>86</v>
       </c>
@@ -1539,8 +1542,11 @@
       <c r="I1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1">
+      <c r="J1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +1575,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1598,7 +1604,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1627,7 +1633,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1656,7 +1662,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1685,7 +1691,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -1743,7 +1749,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -1772,7 +1778,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -1801,7 +1807,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1830,7 +1836,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -1859,7 +1865,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
@@ -1888,7 +1894,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -1917,7 +1923,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
@@ -1946,7 +1952,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -1975,7 +1981,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
@@ -2004,7 +2010,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
@@ -2033,7 +2039,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>52</v>
       </c>
@@ -2062,7 +2068,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>56</v>
       </c>
@@ -2091,7 +2097,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
@@ -2120,7 +2126,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>16</v>
       </c>
@@ -2149,7 +2155,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>113</v>
       </c>
@@ -2178,7 +2184,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>114</v>
       </c>
@@ -2207,7 +2213,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>115</v>
       </c>
@@ -2236,7 +2242,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>116</v>
       </c>
@@ -2265,7 +2271,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>117</v>
       </c>
@@ -2294,7 +2300,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>140</v>
       </c>
@@ -2323,7 +2329,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>141</v>
       </c>
@@ -2352,7 +2358,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>142</v>
       </c>
@@ -2381,7 +2387,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>143</v>
       </c>
@@ -2410,7 +2416,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>144</v>
       </c>
@@ -2439,7 +2445,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>145</v>
       </c>
@@ -2468,7 +2474,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>146</v>
       </c>
@@ -2497,7 +2503,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>147</v>
       </c>
@@ -2526,7 +2532,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>148</v>
       </c>
@@ -2555,7 +2561,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="22.5">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>149</v>
       </c>
@@ -2584,7 +2590,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>150</v>
       </c>
@@ -2613,7 +2619,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="22.5">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="19" t="s">
         <v>155</v>
       </c>
@@ -2642,7 +2648,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="19" t="s">
         <v>208</v>
       </c>
@@ -2671,7 +2677,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="19" t="s">
         <v>209</v>
       </c>
@@ -2700,7 +2706,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="19" t="s">
         <v>210</v>
       </c>
@@ -2729,7 +2735,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="19" t="s">
         <v>211</v>
       </c>
@@ -2758,7 +2764,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="19" t="s">
         <v>212</v>
       </c>
@@ -2787,7 +2793,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="19" t="s">
         <v>213</v>
       </c>
@@ -2816,7 +2822,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="19" t="s">
         <v>214</v>
       </c>
@@ -2845,7 +2851,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="19" t="s">
         <v>215</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="19" t="s">
         <v>216</v>
       </c>
@@ -2903,7 +2909,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="19" t="s">
         <v>217</v>
       </c>
@@ -2932,7 +2938,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="19" t="s">
         <v>218</v>
       </c>
@@ -2961,7 +2967,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="19" t="s">
         <v>219</v>
       </c>
@@ -2990,7 +2996,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="19" t="s">
         <v>220</v>
       </c>
@@ -3019,7 +3025,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="19" t="s">
         <v>221</v>
       </c>
@@ -3048,7 +3054,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="19" t="s">
         <v>222</v>
       </c>
@@ -3077,7 +3083,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="19" t="s">
         <v>223</v>
       </c>
@@ -3106,7 +3112,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="19" t="s">
         <v>224</v>
       </c>
@@ -3135,7 +3141,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="19" t="s">
         <v>225</v>
       </c>
@@ -3164,7 +3170,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="19" t="s">
         <v>226</v>
       </c>
@@ -3193,7 +3199,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="19" t="s">
         <v>227</v>
       </c>
@@ -3222,7 +3228,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="19" t="s">
         <v>228</v>
       </c>
@@ -3251,7 +3257,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="19" t="s">
         <v>229</v>
       </c>
@@ -3280,7 +3286,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="19" t="s">
         <v>230</v>
       </c>
@@ -3317,12 +3323,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3543,15 +3546,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4F5669-9080-4211-AAB2-07BF8DFB6BC3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2A8D83-3442-4B82-A652-52EBAFE721A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cee211f1-5bf1-4f4b-adf1-18b7c5b9a3a6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3576,17 +3590,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2A8D83-3442-4B82-A652-52EBAFE721A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4F5669-9080-4211-AAB2-07BF8DFB6BC3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cee211f1-5bf1-4f4b-adf1-18b7c5b9a3a6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixing issues that arrose after branch merge with GPW13/billionaiRe-master and PR
</commit_message>
<xml_diff>
--- a/data-raw/indicator_order.xlsx
+++ b/data-raw/indicator_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8FD295-B5E5-428A-8395-D5CA4962607E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0B30CE-2C59-4B23-B80E-224543054486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{BB7C0A8F-3E4B-42D2-A48C-0464F3997827}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="278">
   <si>
     <t>SDG 2.2.1</t>
   </si>
@@ -964,9 +964,6 @@
   </si>
   <si>
     <t>detect_response</t>
-  </si>
-  <si>
-    <t>comment</t>
   </si>
 </sst>
 </file>
@@ -1497,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497A527C-AEDB-4138-8664-DD03992C96A6}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1514,7 +1511,7 @@
     <col min="8" max="8" width="9.1796875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>86</v>
       </c>
@@ -1542,11 +1539,8 @@
       <c r="I1" t="s">
         <v>268</v>
       </c>
-      <c r="J1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +1569,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1604,7 +1598,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1633,7 +1627,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1662,7 +1656,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1691,7 +1685,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1720,7 +1714,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -1749,7 +1743,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -1778,7 +1772,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -1807,7 +1801,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1836,7 +1830,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -1865,7 +1859,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
@@ -1894,7 +1888,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -1923,7 +1917,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
@@ -1952,7 +1946,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -3323,12 +3317,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -3545,6 +3533,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3555,22 +3549,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2A8D83-3442-4B82-A652-52EBAFE721A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cee211f1-5bf1-4f4b-adf1-18b7c5b9a3a6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C331FB4-7C5E-4701-8F41-17478B6D46F4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3589,6 +3567,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2A8D83-3442-4B82-A652-52EBAFE721A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cee211f1-5bf1-4f4b-adf1-18b7c5b9a3a6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4F5669-9080-4211-AAB2-07BF8DFB6BC3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Finalizing HEP country summaries, fixing compabilities when _all functions used. Finalizing country summaries for all billions.
</commit_message>
<xml_diff>
--- a/data-raw/indicator_order.xlsx
+++ b/data-raw/indicator_order.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0B30CE-2C59-4B23-B80E-224543054486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A83178-B0AA-4B7D-B858-6B3DB423414E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{BB7C0A8F-3E4B-42D2-A48C-0464F3997827}"/>
+    <workbookView xWindow="32280" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{BB7C0A8F-3E4B-42D2-A48C-0464F3997827}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="285">
   <si>
     <t>SDG 2.2.1</t>
   </si>
@@ -963,14 +963,35 @@
     <t>prevent</t>
   </si>
   <si>
-    <t>detect_response</t>
+    <t>hep_idx</t>
+  </si>
+  <si>
+    <t>HEPI</t>
+  </si>
+  <si>
+    <t>HEP index</t>
+  </si>
+  <si>
+    <t>DECREP4</t>
+  </si>
+  <si>
+    <t>Time to detect and respond</t>
+  </si>
+  <si>
+    <t>PREV8</t>
+  </si>
+  <si>
+    <t>Prevent</t>
+  </si>
+  <si>
+    <t>respond</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1115,7 +1136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1179,6 +1200,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1494,24 +1518,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497A527C-AEDB-4138-8664-DD03992C96A6}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="D38" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="28.7265625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="86.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.7265625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="33.81640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="11"/>
+    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="28.77734375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="86.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.77734375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="33.77734375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="9" t="s">
         <v>86</v>
       </c>
@@ -1540,7 +1564,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="4" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +1593,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1598,7 +1622,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1627,7 +1651,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1656,7 +1680,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1685,7 +1709,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1714,7 +1738,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -1743,7 +1767,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -1772,7 +1796,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -1801,7 +1825,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1830,7 +1854,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -1853,13 +1877,13 @@
         <v>90</v>
       </c>
       <c r="H12" s="11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
@@ -1882,13 +1906,13 @@
         <v>99</v>
       </c>
       <c r="H13" s="11">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -1911,13 +1935,13 @@
         <v>94</v>
       </c>
       <c r="H14" s="11">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
@@ -1940,13 +1964,13 @@
         <v>88</v>
       </c>
       <c r="H15" s="11">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -1969,13 +1993,13 @@
         <v>104</v>
       </c>
       <c r="H16" s="11">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
@@ -1998,13 +2022,13 @@
         <v>78</v>
       </c>
       <c r="H17" s="11">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
@@ -2027,13 +2051,13 @@
         <v>73</v>
       </c>
       <c r="H18" s="11">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
         <v>52</v>
       </c>
@@ -2056,13 +2080,13 @@
         <v>67</v>
       </c>
       <c r="H19" s="11">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
         <v>56</v>
       </c>
@@ -2085,13 +2109,13 @@
         <v>75</v>
       </c>
       <c r="H20" s="11">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9">
       <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
@@ -2114,13 +2138,13 @@
         <v>79</v>
       </c>
       <c r="H21" s="11">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9">
       <c r="A22" s="6" t="s">
         <v>16</v>
       </c>
@@ -2143,13 +2167,13 @@
         <v>81</v>
       </c>
       <c r="H22" s="11">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9">
       <c r="A23" s="7" t="s">
         <v>113</v>
       </c>
@@ -2172,13 +2196,13 @@
         <v>156</v>
       </c>
       <c r="H23" s="11">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I23" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9">
       <c r="A24" s="7" t="s">
         <v>114</v>
       </c>
@@ -2201,13 +2225,13 @@
         <v>159</v>
       </c>
       <c r="H24" s="11">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I24" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9">
       <c r="A25" s="7" t="s">
         <v>115</v>
       </c>
@@ -2230,13 +2254,13 @@
         <v>160</v>
       </c>
       <c r="H25" s="11">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I25" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="A26" s="7" t="s">
         <v>116</v>
       </c>
@@ -2259,13 +2283,13 @@
         <v>163</v>
       </c>
       <c r="H26" s="11">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I26" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9">
       <c r="A27" s="7" t="s">
         <v>117</v>
       </c>
@@ -2288,13 +2312,13 @@
         <v>161</v>
       </c>
       <c r="H27" s="11">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I27" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9">
       <c r="A28" s="7" t="s">
         <v>140</v>
       </c>
@@ -2317,13 +2341,13 @@
         <v>164</v>
       </c>
       <c r="H28" s="11">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I28" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9">
       <c r="A29" s="7" t="s">
         <v>141</v>
       </c>
@@ -2346,13 +2370,13 @@
         <v>165</v>
       </c>
       <c r="H29" s="11">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I29" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9">
       <c r="A30" s="7" t="s">
         <v>142</v>
       </c>
@@ -2375,13 +2399,13 @@
         <v>166</v>
       </c>
       <c r="H30" s="11">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I30" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9">
       <c r="A31" s="7" t="s">
         <v>143</v>
       </c>
@@ -2404,13 +2428,13 @@
         <v>167</v>
       </c>
       <c r="H31" s="11">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I31" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9">
       <c r="A32" s="7" t="s">
         <v>144</v>
       </c>
@@ -2433,13 +2457,13 @@
         <v>168</v>
       </c>
       <c r="H32" s="11">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I32" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9">
       <c r="A33" s="7" t="s">
         <v>145</v>
       </c>
@@ -2462,13 +2486,13 @@
         <v>169</v>
       </c>
       <c r="H33" s="11">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I33" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9">
       <c r="A34" s="7" t="s">
         <v>146</v>
       </c>
@@ -2491,13 +2515,13 @@
         <v>170</v>
       </c>
       <c r="H34" s="11">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I34" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9">
       <c r="A35" s="7" t="s">
         <v>147</v>
       </c>
@@ -2520,13 +2544,13 @@
         <v>171</v>
       </c>
       <c r="H35" s="11">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I35" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9">
       <c r="A36" s="7" t="s">
         <v>148</v>
       </c>
@@ -2549,13 +2573,13 @@
         <v>158</v>
       </c>
       <c r="H36" s="11">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I36" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="20.399999999999999">
       <c r="A37" s="7" t="s">
         <v>149</v>
       </c>
@@ -2578,13 +2602,13 @@
         <v>157</v>
       </c>
       <c r="H37" s="11">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I37" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9">
       <c r="A38" s="7" t="s">
         <v>150</v>
       </c>
@@ -2607,13 +2631,13 @@
         <v>172</v>
       </c>
       <c r="H38" s="11">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I38" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9">
       <c r="A39" s="19" t="s">
         <v>155</v>
       </c>
@@ -2636,13 +2660,13 @@
         <v>162</v>
       </c>
       <c r="H39" s="11">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I39" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9">
       <c r="A40" s="19" t="s">
         <v>208</v>
       </c>
@@ -2665,13 +2689,13 @@
         <v>234</v>
       </c>
       <c r="H40" s="11">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I40" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9">
       <c r="A41" s="19" t="s">
         <v>209</v>
       </c>
@@ -2694,13 +2718,13 @@
         <v>235</v>
       </c>
       <c r="H41" s="11">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I41" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9">
       <c r="A42" s="19" t="s">
         <v>210</v>
       </c>
@@ -2723,13 +2747,13 @@
         <v>236</v>
       </c>
       <c r="H42" s="11">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I42" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9">
       <c r="A43" s="19" t="s">
         <v>211</v>
       </c>
@@ -2752,13 +2776,13 @@
         <v>237</v>
       </c>
       <c r="H43" s="11">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I43" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9">
       <c r="A44" s="19" t="s">
         <v>212</v>
       </c>
@@ -2781,13 +2805,13 @@
         <v>238</v>
       </c>
       <c r="H44" s="11">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I44" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9">
       <c r="A45" s="19" t="s">
         <v>213</v>
       </c>
@@ -2810,13 +2834,13 @@
         <v>239</v>
       </c>
       <c r="H45" s="11">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="I45" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9">
       <c r="A46" s="19" t="s">
         <v>214</v>
       </c>
@@ -2839,13 +2863,13 @@
         <v>240</v>
       </c>
       <c r="H46" s="11">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I46" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9">
       <c r="A47" s="19" t="s">
         <v>215</v>
       </c>
@@ -2868,13 +2892,13 @@
         <v>241</v>
       </c>
       <c r="H47" s="11">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I47" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9">
       <c r="A48" s="19" t="s">
         <v>216</v>
       </c>
@@ -2897,13 +2921,13 @@
         <v>242</v>
       </c>
       <c r="H48" s="11">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I48" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9">
       <c r="A49" s="19" t="s">
         <v>217</v>
       </c>
@@ -2926,13 +2950,13 @@
         <v>243</v>
       </c>
       <c r="H49" s="11">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I49" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9">
       <c r="A50" s="19" t="s">
         <v>218</v>
       </c>
@@ -2955,13 +2979,13 @@
         <v>244</v>
       </c>
       <c r="H50" s="11">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I50" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9">
       <c r="A51" s="19" t="s">
         <v>219</v>
       </c>
@@ -2984,13 +3008,13 @@
         <v>245</v>
       </c>
       <c r="H51" s="11">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I51" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9">
       <c r="A52" s="19" t="s">
         <v>220</v>
       </c>
@@ -3013,13 +3037,13 @@
         <v>246</v>
       </c>
       <c r="H52" s="11">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I52" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9">
       <c r="A53" s="19" t="s">
         <v>221</v>
       </c>
@@ -3042,13 +3066,13 @@
         <v>247</v>
       </c>
       <c r="H53" s="11">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="I53" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9">
       <c r="A54" s="19" t="s">
         <v>222</v>
       </c>
@@ -3071,13 +3095,13 @@
         <v>248</v>
       </c>
       <c r="H54" s="11">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I54" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9">
       <c r="A55" s="19" t="s">
         <v>223</v>
       </c>
@@ -3100,13 +3124,13 @@
         <v>250</v>
       </c>
       <c r="H55" s="11">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I55" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9">
       <c r="A56" s="19" t="s">
         <v>224</v>
       </c>
@@ -3129,13 +3153,13 @@
         <v>251</v>
       </c>
       <c r="H56" s="11">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="I56" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9">
       <c r="A57" s="19" t="s">
         <v>225</v>
       </c>
@@ -3158,13 +3182,13 @@
         <v>252</v>
       </c>
       <c r="H57" s="11">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="I57" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9">
       <c r="A58" s="19" t="s">
         <v>226</v>
       </c>
@@ -3187,13 +3211,13 @@
         <v>253</v>
       </c>
       <c r="H58" s="11">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I58" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9">
       <c r="A59" s="19" t="s">
         <v>227</v>
       </c>
@@ -3216,76 +3240,76 @@
         <v>254</v>
       </c>
       <c r="H59" s="11">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I59" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9">
       <c r="A60" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H60" s="11">
+        <v>59</v>
+      </c>
+      <c r="I60" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B61" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="C60" s="20" t="s">
+      <c r="C61" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="D60" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="E60" s="20" t="s">
+      <c r="D61" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="E61" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="F60" s="20" t="s">
+      <c r="F61" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="G60" s="5" t="s">
+      <c r="G61" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="H60" s="11">
-        <v>55</v>
-      </c>
-      <c r="I60" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61" s="19" t="s">
+      <c r="H61" s="11">
+        <v>60</v>
+      </c>
+      <c r="I61" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B61" s="21" t="s">
+      <c r="B62" s="21" t="s">
         <v>186</v>
-      </c>
-      <c r="C61" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="E61" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="F61" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="H61" s="11">
-        <v>56</v>
-      </c>
-      <c r="I61" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="B62" s="21" t="s">
-        <v>187</v>
       </c>
       <c r="C62" s="21" t="s">
         <v>265</v>
@@ -3294,19 +3318,106 @@
         <v>258</v>
       </c>
       <c r="E62" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="F62" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="H62" s="11">
+        <v>61</v>
+      </c>
+      <c r="I62" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="B63" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="F62" s="21" t="s">
+      <c r="C63" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="E63" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="G62" s="5" t="s">
+      <c r="F63" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="H63" s="11">
+        <v>62</v>
+      </c>
+      <c r="I63" t="s">
         <v>256</v>
       </c>
-      <c r="H62" s="11">
-        <v>57</v>
-      </c>
-      <c r="I62" t="s">
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="B64" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="H64" s="11">
+        <v>63</v>
+      </c>
+      <c r="I64" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="G65" s="5" t="s">
         <v>277</v>
+      </c>
+      <c r="H65" s="11">
+        <v>64</v>
+      </c>
+      <c r="I65" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -3317,6 +3428,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -3533,22 +3659,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2A8D83-3442-4B82-A652-52EBAFE721A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cee211f1-5bf1-4f4b-adf1-18b7c5b9a3a6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4F5669-9080-4211-AAB2-07BF8DFB6BC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C331FB4-7C5E-4701-8F41-17478B6D46F4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3565,28 +3700,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C2A8D83-3442-4B82-A652-52EBAFE721A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cee211f1-5bf1-4f4b-adf1-18b7c5b9a3a6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4F5669-9080-4211-AAB2-07BF8DFB6BC3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>